<commit_message>
5 new words mastered
</commit_message>
<xml_diff>
--- a/hsk4_vocabulary.xlsx
+++ b/hsk4_vocabulary.xlsx
@@ -20764,7 +20764,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21691,6 +21691,106 @@
       <c r="D46" t="inlineStr">
         <is>
           <t>simple</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>463</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>经历</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>jīnglì</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>experience</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1119</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>真</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>zhēn</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>really</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>889</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>网球</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>wǎngqiú</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Tennis</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>195</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>动作</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>dòngzuò</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>action</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>785</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>手表</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>shǒubiǎo</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Wrist Watch</t>
         </is>
       </c>
     </row>
@@ -21737,101 +21837,101 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>852</v>
+        <v>463</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>提供</t>
+          <t>经历</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>tígōng</t>
+          <t>jīnglì</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>provide</t>
+          <t>experience</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>458</v>
+        <v>1119</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>精神</t>
+          <t>真</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>jīngshén</t>
+          <t>zhēn</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>spirit</t>
+          <t>really</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>651</v>
+        <v>889</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>啤酒</t>
+          <t>网球</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>píjiǔ</t>
+          <t>wǎngqiú</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Beer</t>
+          <t>Tennis</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>446</v>
+        <v>195</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>解决</t>
+          <t>动作</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>jiějué</t>
+          <t>dòngzuò</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Solve</t>
+          <t>action</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>414</v>
+        <v>785</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>简单</t>
+          <t>手表</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>jiǎndān</t>
+          <t>shǒubiǎo</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>simple</t>
+          <t>Wrist Watch</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 5 another words to "przerobione"
</commit_message>
<xml_diff>
--- a/hsk4_vocabulary.xlsx
+++ b/hsk4_vocabulary.xlsx
@@ -20764,7 +20764,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21791,6 +21791,106 @@
       <c r="D51" t="inlineStr">
         <is>
           <t>Wrist Watch</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>183</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>电视</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>diànshì</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>television</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>801</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>数字</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>shùzì</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>126</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>聪明</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>cōngming</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>clever</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>501</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>刻</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>kè</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>moment</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>962</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>辛苦</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>xīnkǔ</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>hard</t>
         </is>
       </c>
     </row>
@@ -21837,101 +21937,101 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>463</v>
+        <v>183</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>经历</t>
+          <t>电视</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>jīnglì</t>
+          <t>diànshì</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>experience</t>
+          <t>television</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1119</v>
+        <v>801</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>真</t>
+          <t>数字</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>zhēn</t>
+          <t>shùzì</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>really</t>
+          <t>number</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>889</v>
+        <v>126</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>网球</t>
+          <t>聪明</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>wǎngqiú</t>
+          <t>cōngming</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Tennis</t>
+          <t>clever</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>195</v>
+        <v>501</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>动作</t>
+          <t>刻</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dòngzuò</t>
+          <t>kè</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>action</t>
+          <t>moment</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>785</v>
+        <v>962</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>手表</t>
+          <t>辛苦</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>shǒubiǎo</t>
+          <t>xīnkǔ</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Wrist Watch</t>
+          <t>hard</t>
         </is>
       </c>
     </row>

</xml_diff>